<commit_message>
Added LoginTest file, TestBase file and accordingly modified other pages files
</commit_message>
<xml_diff>
--- a/resources/testdata/data.xlsx
+++ b/resources/testdata/data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CreateAccount" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidLogin" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Email</t>
   </si>
@@ -101,6 +102,36 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>automation06@gmail.com</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>Password is required.</t>
+  </si>
+  <si>
+    <t>An email address required.</t>
+  </si>
+  <si>
+    <t>Authentication failed.</t>
+  </si>
+  <si>
+    <t>autom@gmail.com</t>
+  </si>
+  <si>
+    <t>automation@gmail</t>
+  </si>
+  <si>
+    <t>auto123</t>
+  </si>
+  <si>
+    <t>Invalid email address.</t>
+  </si>
+  <si>
+    <t>123Auto</t>
   </si>
 </sst>
 </file>
@@ -442,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="15"/>
@@ -562,14 +593,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>